<commit_message>
make h2gc to h2 available and change transport of h2
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_SUP_Refineries_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_SUP_Refineries_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1C2753-BE10-485D-84EF-DE1C028BA6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9094541E-CCCC-4367-906F-0D024D59387A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16356" yWindow="1560" windowWidth="21012" windowHeight="14256" tabRatio="733" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17052" yWindow="2256" windowWidth="21012" windowHeight="14256" tabRatio="733" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="11" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>SUPH2PEMC2N</t>
+  </si>
+  <si>
+    <t>DELH2GC</t>
   </si>
 </sst>
 </file>
@@ -25659,7 +25662,7 @@
   <dimension ref="B3:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -25808,11 +25811,21 @@
       </c>
     </row>
     <row r="11" spans="2:10">
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="24"/>
+      <c r="F11" s="11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="11">
+        <v>1</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix name of region bornholm in refierneries trans file
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_SUP_Refineries_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_SUP_Refineries_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9094541E-CCCC-4367-906F-0D024D59387A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B1E5DC-0D89-49F3-8738-CC284FAA978A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17052" yWindow="2256" windowWidth="21012" windowHeight="14256" tabRatio="733" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17100" yWindow="2100" windowWidth="21012" windowHeight="14256" tabRatio="733" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="11" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>AllRegions</t>
   </si>
   <si>
-    <t>DHISLBH</t>
-  </si>
-  <si>
     <t>DKISL1</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>DELH2GC</t>
+  </si>
+  <si>
+    <t>DKISLBH</t>
   </si>
 </sst>
 </file>
@@ -25662,7 +25662,7 @@
   <dimension ref="B3:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -25690,16 +25690,16 @@
         <v>12</v>
       </c>
       <c r="F4" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="H4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="I4" s="22" t="s">
         <v>17</v>
-      </c>
-      <c r="I4" s="22" t="s">
-        <v>18</v>
       </c>
       <c r="J4" s="23" t="s">
         <v>10</v>
@@ -25722,7 +25722,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:10">
@@ -25739,7 +25739,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:10">
@@ -25756,7 +25756,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:10">
@@ -25773,7 +25773,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:10">
@@ -25790,7 +25790,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:10">
@@ -25807,7 +25807,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:10">
@@ -25824,7 +25824,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make Ammonia, Methanol and Jet Fuel Production available
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_SUP_Refineries_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_SUP_Refineries_Trans.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B1E5DC-0D89-49F3-8738-CC284FAA978A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1266FCCA-1CD9-44A5-91A4-E9AD1732B5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17100" yWindow="2100" windowWidth="21012" windowHeight="14256" tabRatio="733" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5070" windowWidth="38430" windowHeight="10500" tabRatio="733" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="11" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -164,12 +164,24 @@
   <si>
     <t>DKISLBH</t>
   </si>
+  <si>
+    <t>SUPELCAMM01</t>
+  </si>
+  <si>
+    <t>SUPMOECO2C1</t>
+  </si>
+  <si>
+    <t>SUPKRECO2C1</t>
+  </si>
+  <si>
+    <t>SUPKRECO2C2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="12">
+  <numFmts count="13">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
@@ -182,8 +194,9 @@
     <numFmt numFmtId="171" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="172" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
     <numFmt numFmtId="173" formatCode="0_ ;\-0\ "/>
+    <numFmt numFmtId="174" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="60">
+  <fonts count="61">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,6 +580,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="68">
     <fill>
@@ -938,7 +956,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1150,6 +1168,15 @@
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -5785,7 +5812,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5835,6 +5862,9 @@
     <xf numFmtId="0" fontId="55" fillId="67" borderId="16" xfId="1325" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1325" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4493"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="4493" applyBorder="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="4493" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4494">
     <cellStyle name="_x000a_shell=progma 2" xfId="656" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -25027,13 +25057,13 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="172.88671875" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="172.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">
@@ -25621,34 +25651,34 @@
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
     </row>
-    <row r="71" spans="1:5" ht="15.6">
+    <row r="71" spans="1:5" ht="15.75">
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:5" ht="15.6">
+    <row r="72" spans="1:5" ht="15.75">
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:5" ht="15.6">
+    <row r="73" spans="1:5" ht="15.75">
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:5" ht="15.6">
+    <row r="74" spans="1:5" ht="15.75">
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="1:5" ht="15.6">
+    <row r="75" spans="1:5" ht="15.75">
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:5" ht="15.6">
+    <row r="76" spans="1:5" ht="15.75">
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:5" ht="15.6">
+    <row r="77" spans="1:5" ht="15.75">
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:5" ht="15.6">
+    <row r="78" spans="1:5" ht="15.75">
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:5" ht="15.6">
+    <row r="79" spans="1:5" ht="15.75">
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:5" ht="15.6">
+    <row r="80" spans="1:5" ht="15.75">
       <c r="D80" s="3"/>
     </row>
   </sheetData>
@@ -25659,13 +25689,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EF56F5-FFEC-4195-B835-F2DA1F364DE3}">
-  <dimension ref="B3:J11"/>
+  <dimension ref="B3:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="2:10">
       <c r="B3" s="19" t="s">
@@ -25676,7 +25706,7 @@
       <c r="E3" s="20"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="2:10" ht="15" thickBot="1">
+    <row r="4" spans="2:10" ht="15.75" thickBot="1">
       <c r="B4" s="21" t="s">
         <v>9</v>
       </c>
@@ -25810,7 +25840,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" ht="15.75" thickBot="1">
       <c r="F11" s="11">
         <v>1</v>
       </c>
@@ -25827,6 +25857,82 @@
         <v>24</v>
       </c>
     </row>
+    <row r="12" spans="2:10">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="11">
+        <v>1</v>
+      </c>
+      <c r="H12" s="11">
+        <v>1</v>
+      </c>
+      <c r="I12" s="11">
+        <v>1</v>
+      </c>
+      <c r="J12" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="16.5">
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+      <c r="G13" s="11">
+        <v>1</v>
+      </c>
+      <c r="H13" s="11">
+        <v>1</v>
+      </c>
+      <c r="I13" s="11">
+        <v>1</v>
+      </c>
+      <c r="J13" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="16.5">
+      <c r="F14" s="11">
+        <v>1</v>
+      </c>
+      <c r="G14" s="11">
+        <v>1</v>
+      </c>
+      <c r="H14" s="11">
+        <v>1</v>
+      </c>
+      <c r="I14" s="11">
+        <v>1</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="F15" s="11">
+        <v>1</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+      <c r="H15" s="11">
+        <v>1</v>
+      </c>
+      <c r="I15" s="11">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="10:12">
+      <c r="J18" s="27"/>
+      <c r="L18" s="27"/>
+    </row>
+    <row r="19" spans="10:12">
+      <c r="J19" s="27"/>
+      <c r="L19" s="27"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Make Rural electrolysis facilities available in all the regions
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_SUP_Refineries_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_SUP_Refineries_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SubRES_TMPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{1266FCCA-1CD9-44A5-91A4-E9AD1732B5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{757F6CE3-2914-4566-9304-7CD0158F11A5}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{1266FCCA-1CD9-44A5-91A4-E9AD1732B5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{415A6AF5-FC86-425F-B8D8-949742142CC2}"/>
   <bookViews>
-    <workbookView xWindow="51855" yWindow="3150" windowWidth="20760" windowHeight="12180" tabRatio="733" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="16875" windowHeight="10523" tabRatio="733" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="11" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -178,6 +178,21 @@
   </si>
   <si>
     <t>MAR</t>
+  </si>
+  <si>
+    <t>SUPH2ALKR1N</t>
+  </si>
+  <si>
+    <t>SUPH2ALKR2N</t>
+  </si>
+  <si>
+    <t>SUPH2PEMR1N</t>
+  </si>
+  <si>
+    <t>SUPH2PEMR2N</t>
+  </si>
+  <si>
+    <t>SUPH2SOER2N</t>
   </si>
 </sst>
 </file>
@@ -25692,10 +25707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EF56F5-FFEC-4195-B835-F2DA1F364DE3}">
-  <dimension ref="B3:M19"/>
+  <dimension ref="B3:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="101" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -25967,13 +25982,107 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="11:13">
-      <c r="K18" s="27"/>
+    <row r="16" spans="2:11">
+      <c r="F16" s="11">
+        <v>1</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1</v>
+      </c>
+      <c r="H16" s="11">
+        <v>1</v>
+      </c>
+      <c r="I16" s="11">
+        <v>1</v>
+      </c>
+      <c r="J16" s="11">
+        <v>1</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="6:13">
+      <c r="F17" s="11">
+        <v>1</v>
+      </c>
+      <c r="G17" s="11">
+        <v>1</v>
+      </c>
+      <c r="H17" s="11">
+        <v>1</v>
+      </c>
+      <c r="I17" s="11">
+        <v>1</v>
+      </c>
+      <c r="J17" s="11">
+        <v>1</v>
+      </c>
+      <c r="K17" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13">
+      <c r="F18" s="11">
+        <v>1</v>
+      </c>
+      <c r="G18" s="11">
+        <v>1</v>
+      </c>
+      <c r="H18" s="11">
+        <v>1</v>
+      </c>
+      <c r="I18" s="11">
+        <v>1</v>
+      </c>
+      <c r="J18" s="11">
+        <v>1</v>
+      </c>
+      <c r="K18" s="24" t="s">
+        <v>33</v>
+      </c>
       <c r="M18" s="27"/>
     </row>
-    <row r="19" spans="11:13">
-      <c r="K19" s="27"/>
+    <row r="19" spans="6:13">
+      <c r="F19" s="11">
+        <v>1</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1</v>
+      </c>
+      <c r="H19" s="11">
+        <v>1</v>
+      </c>
+      <c r="I19" s="11">
+        <v>1</v>
+      </c>
+      <c r="J19" s="11">
+        <v>1</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="M19" s="27"/>
+    </row>
+    <row r="20" spans="6:13">
+      <c r="F20" s="11">
+        <v>1</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1</v>
+      </c>
+      <c r="H20" s="11">
+        <v>1</v>
+      </c>
+      <c r="I20" s="11">
+        <v>1</v>
+      </c>
+      <c r="J20" s="11">
+        <v>1</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update (again) to make rural production units available
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_SUP_Refineries_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_SUP_Refineries_Trans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1266FCCA-1CD9-44A5-91A4-E9AD1732B5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10BB439-0BE4-40FD-BCEF-BFDC9300BA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5070" windowWidth="38430" windowHeight="10500" tabRatio="733" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17220" yWindow="504" windowWidth="23412" windowHeight="15888" tabRatio="733" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="11" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -175,6 +175,24 @@
   </si>
   <si>
     <t>SUPKRECO2C2</t>
+  </si>
+  <si>
+    <t>SUPELCAMM03</t>
+  </si>
+  <si>
+    <t>SUPH2ALKR1N</t>
+  </si>
+  <si>
+    <t>SUPH2ALKR2N</t>
+  </si>
+  <si>
+    <t>SUPH2PEMR1N</t>
+  </si>
+  <si>
+    <t>SUPH2PEMR2N</t>
+  </si>
+  <si>
+    <t>SUPH2SOER2N</t>
   </si>
 </sst>
 </file>
@@ -25057,13 +25075,13 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="7.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="172.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="172.88671875" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">
@@ -25651,34 +25669,34 @@
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75">
+    <row r="71" spans="1:5" ht="15.6">
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75">
+    <row r="72" spans="1:5" ht="15.6">
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75">
+    <row r="73" spans="1:5" ht="15.6">
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75">
+    <row r="74" spans="1:5" ht="15.6">
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75">
+    <row r="75" spans="1:5" ht="15.6">
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75">
+    <row r="76" spans="1:5" ht="15.6">
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75">
+    <row r="77" spans="1:5" ht="15.6">
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75">
+    <row r="78" spans="1:5" ht="15.6">
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75">
+    <row r="79" spans="1:5" ht="15.6">
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75">
+    <row r="80" spans="1:5" ht="15.6">
       <c r="D80" s="3"/>
     </row>
   </sheetData>
@@ -25689,13 +25707,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EF56F5-FFEC-4195-B835-F2DA1F364DE3}">
-  <dimension ref="B3:L19"/>
+  <dimension ref="B3:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="3" spans="2:10">
       <c r="B3" s="19" t="s">
@@ -25706,7 +25724,7 @@
       <c r="E3" s="20"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1">
+    <row r="4" spans="2:10" ht="15" thickBot="1">
       <c r="B4" s="21" t="s">
         <v>9</v>
       </c>
@@ -25840,7 +25858,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15.75" thickBot="1">
+    <row r="11" spans="2:10" ht="15" thickBot="1">
       <c r="F11" s="11">
         <v>1</v>
       </c>
@@ -25874,7 +25892,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="16.5">
+    <row r="13" spans="2:10">
       <c r="F13" s="11">
         <v>1</v>
       </c>
@@ -25891,7 +25909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="16.5">
+    <row r="14" spans="2:10">
       <c r="F14" s="11">
         <v>1</v>
       </c>
@@ -25908,7 +25926,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" ht="15" thickBot="1">
       <c r="F15" s="11">
         <v>1</v>
       </c>
@@ -25925,13 +25943,112 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="10:12">
-      <c r="J18" s="27"/>
+    <row r="16" spans="2:10">
+      <c r="F16" s="11">
+        <v>1</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1</v>
+      </c>
+      <c r="H16" s="11">
+        <v>1</v>
+      </c>
+      <c r="I16" s="11">
+        <v>1</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12">
+      <c r="F17" s="11">
+        <v>1</v>
+      </c>
+      <c r="G17" s="11">
+        <v>1</v>
+      </c>
+      <c r="H17" s="11">
+        <v>1</v>
+      </c>
+      <c r="I17" s="11">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="6:12">
+      <c r="F18" s="11">
+        <v>1</v>
+      </c>
+      <c r="G18" s="11">
+        <v>1</v>
+      </c>
+      <c r="H18" s="11">
+        <v>1</v>
+      </c>
+      <c r="I18" s="11">
+        <v>1</v>
+      </c>
+      <c r="J18" s="27" t="s">
+        <v>32</v>
+      </c>
       <c r="L18" s="27"/>
     </row>
-    <row r="19" spans="10:12">
-      <c r="J19" s="27"/>
+    <row r="19" spans="6:12">
+      <c r="F19" s="11">
+        <v>1</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1</v>
+      </c>
+      <c r="H19" s="11">
+        <v>1</v>
+      </c>
+      <c r="I19" s="11">
+        <v>1</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>33</v>
+      </c>
       <c r="L19" s="27"/>
+    </row>
+    <row r="20" spans="6:12">
+      <c r="F20" s="11">
+        <v>1</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1</v>
+      </c>
+      <c r="H20" s="11">
+        <v>1</v>
+      </c>
+      <c r="I20" s="11">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="6:12">
+      <c r="F21" s="11">
+        <v>1</v>
+      </c>
+      <c r="G21" s="11">
+        <v>1</v>
+      </c>
+      <c r="H21" s="11">
+        <v>1</v>
+      </c>
+      <c r="I21" s="11">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="6:12">
+      <c r="J22" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>